<commit_message>
added optional salt in addition to default salt
</commit_message>
<xml_diff>
--- a/example_consent_anonymized.xlsx
+++ b/example_consent_anonymized.xlsx
@@ -31,10 +31,10 @@
     <t>semester</t>
   </si>
   <si>
-    <t>MUXklTc2QuWZWY7SEpvCNDnSl7U=</t>
-  </si>
-  <si>
-    <t>EE6omAvwQSMQmmhYVhBkWVmHq8M=</t>
+    <t>kWVo-vt4JQka9F6c5qtT7NYkj_A=</t>
+  </si>
+  <si>
+    <t>i32JKUsm7lIJ7ceMpSkZHlKq9cE=</t>
   </si>
   <si>
     <t>YES</t>

</xml_diff>